<commit_message>
Actualización de IP a servidores
</commit_message>
<xml_diff>
--- a/DOCUMENTOS GENERALES/Servicios.xlsx
+++ b/DOCUMENTOS GENERALES/Servicios.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\All-documents\DOCUMENTOS GENERALES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="BD" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="191">
   <si>
     <t>Nombre</t>
   </si>
@@ -575,12 +575,39 @@
   </si>
   <si>
     <t>https://github.com/aagarcia25/sicsa</t>
+  </si>
+  <si>
+    <t>nueva ip</t>
+  </si>
+  <si>
+    <t>10.210.26.26</t>
+  </si>
+  <si>
+    <t>10.210.26.25</t>
+  </si>
+  <si>
+    <t>10.210.26.27</t>
+  </si>
+  <si>
+    <t>10.210.0.30</t>
+  </si>
+  <si>
+    <t>10.210.26.28</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>NAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -709,7 +736,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -935,40 +965,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:G23" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:G23" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:G23"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Ambiente" dataDxfId="14"/>
-    <tableColumn id="8" name="Tipo" dataDxfId="13"/>
-    <tableColumn id="2" name="Permiso" dataDxfId="12"/>
-    <tableColumn id="3" name="NombreSesión" dataDxfId="11"/>
-    <tableColumn id="4" name="IP" dataDxfId="10"/>
-    <tableColumn id="6" name="Usuario BD" dataDxfId="9"/>
-    <tableColumn id="7" name="Contraseña" dataDxfId="8"/>
+    <tableColumn id="1" name="Ambiente" dataDxfId="15"/>
+    <tableColumn id="8" name="Tipo" dataDxfId="14"/>
+    <tableColumn id="2" name="Permiso" dataDxfId="13"/>
+    <tableColumn id="3" name="NombreSesión" dataDxfId="12"/>
+    <tableColumn id="4" name="IP" dataDxfId="11"/>
+    <tableColumn id="6" name="Usuario BD" dataDxfId="10"/>
+    <tableColumn id="7" name="Contraseña" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:Q12" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:Q12"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:R12" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:R12"/>
+  <tableColumns count="18">
     <tableColumn id="1" name="Ambiente"/>
     <tableColumn id="2" name="Conexión"/>
     <tableColumn id="3" name="Permiso"/>
     <tableColumn id="4" name="Nombre"/>
-    <tableColumn id="5" name="Puerto" dataDxfId="6"/>
-    <tableColumn id="6" name="IP" dataDxfId="5"/>
+    <tableColumn id="5" name="Puerto" dataDxfId="7"/>
+    <tableColumn id="6" name="IP" dataDxfId="6"/>
+    <tableColumn id="14" name="nueva ip" dataDxfId="0"/>
     <tableColumn id="7" name="Host"/>
     <tableColumn id="8" name="Usuario"/>
     <tableColumn id="9" name="Contraseña"/>
     <tableColumn id="10" name="RAM"/>
     <tableColumn id="11" name="Núcleos"/>
     <tableColumn id="12" name="SO"/>
-    <tableColumn id="13" name="Version" dataDxfId="4"/>
-    <tableColumn id="20" name="Interno" dataDxfId="3"/>
-    <tableColumn id="19" name="Externo" dataDxfId="2"/>
+    <tableColumn id="13" name="Version" dataDxfId="5"/>
+    <tableColumn id="20" name="Interno" dataDxfId="4"/>
+    <tableColumn id="19" name="Externo" dataDxfId="3"/>
     <tableColumn id="15" name="Procesador"/>
     <tableColumn id="18" name="Equipo"/>
   </tableColumns>
@@ -984,7 +1015,7 @@
     <tableColumn id="2" name="Ambiente" dataCellStyle="Normal"/>
     <tableColumn id="11" name="Nombre Corto" dataCellStyle="Normal"/>
     <tableColumn id="3" name="IP" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Puerto" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Puerto" dataDxfId="2" dataCellStyle="Normal"/>
     <tableColumn id="5" name="Estatus" dataCellStyle="Normal"/>
     <tableColumn id="6" name="Descripcion" dataCellStyle="Normal"/>
     <tableColumn id="7" name="Repositorio" dataCellStyle="Normal"/>
@@ -995,7 +1026,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A1:B8" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A1:B8" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:B8"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Tiempo"/>
@@ -1273,9 +1304,9 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1835,11 +1866,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1849,21 +1880,22 @@
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="9" customFormat="1">
+    <row r="1" spans="1:18" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -1883,40 +1915,43 @@
         <v>1</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1935,22 +1970,23 @@
       <c r="F2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>166</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="15">
+      <c r="N2" s="15">
         <v>7</v>
       </c>
-      <c r="N2" s="15"/>
       <c r="O2" s="15"/>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="P2" s="15"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1969,20 +2005,21 @@
       <c r="F3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>39</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2001,20 +2038,21 @@
       <c r="F4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" s="2"/>
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>40</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -2033,23 +2071,24 @@
       <c r="F5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" s="2"/>
+      <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>48</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="3">
         <v>7</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -2068,32 +2107,33 @@
       <c r="F6" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" s="10"/>
+      <c r="I6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>83</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>84</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>4</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="3">
+      <c r="N6" s="3">
         <v>7</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -2112,32 +2152,33 @@
       <c r="F7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" s="2"/>
+      <c r="I7" t="s">
         <v>10</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>167</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>84</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>4</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="3">
+      <c r="N7" s="3">
         <v>7</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -2156,20 +2197,21 @@
       <c r="F8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="2"/>
+      <c r="I8" t="s">
         <v>10</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>93</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>46</v>
       </c>
-      <c r="M8" s="3">
+      <c r="N8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -2188,26 +2230,29 @@
       <c r="F9" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="I9" t="s">
         <v>10</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>95</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="3">
+      <c r="N9" s="3">
         <v>7</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="Q9" s="12" t="s">
+      <c r="R9" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -2226,26 +2271,29 @@
       <c r="F10" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="I10" t="s">
         <v>10</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>95</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="3">
+      <c r="N10" s="3">
         <v>7</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="Q10" s="12" t="s">
+      <c r="R10" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -2264,26 +2312,49 @@
       <c r="F11" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H11" t="s">
+      <c r="G11" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="I11" t="s">
         <v>10</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>95</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="3">
+      <c r="N11" s="3">
         <v>7</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="O11" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="Q11" s="12" t="s">
+      <c r="R11" s="12" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="D12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" t="s">
+        <v>187</v>
+      </c>
+      <c r="I12" t="s">
+        <v>188</v>
+      </c>
+      <c r="J12" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2304,7 +2375,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>